<commit_message>
Added rows / columns of individual names.
</commit_message>
<xml_diff>
--- a/covariance-matrix.xlsx
+++ b/covariance-matrix.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5300" yWindow="1180" windowWidth="23500" windowHeight="15160" tabRatio="500"/>
+    <workbookView xWindow="4720" yWindow="1180" windowWidth="28160" windowHeight="15840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,52 +29,121 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="113">
   <si>
-    <t>ANWC100</t>
+    <t>WAM63</t>
   </si>
   <si>
-    <t>ANWC101</t>
+    <t>WAM60</t>
   </si>
   <si>
-    <t>ANWC102</t>
+    <t>WAM57</t>
   </si>
   <si>
-    <t>ANWC103</t>
+    <t>WAM56</t>
   </si>
   <si>
-    <t>ANWC104</t>
+    <t>WAM55</t>
   </si>
   <si>
-    <t>ANWC105</t>
+    <t>SAM46</t>
   </si>
   <si>
-    <t>ANWC106</t>
+    <t>SAM8</t>
   </si>
   <si>
-    <t>ANWC107</t>
+    <t>SAM44</t>
   </si>
   <si>
-    <t>ANWC108</t>
+    <t>SAM41</t>
   </si>
   <si>
-    <t>ANWC109</t>
+    <t>SAM36</t>
   </si>
   <si>
-    <t>ANWC110</t>
+    <t>WAM64</t>
   </si>
   <si>
-    <t>ANWC112</t>
+    <t>SAM30</t>
   </si>
   <si>
-    <t>ANWC113</t>
+    <t>SAM29</t>
   </si>
   <si>
-    <t>ANWC115</t>
+    <t>SAM28</t>
   </si>
   <si>
-    <t>ANWC116</t>
+    <t>SAM27</t>
   </si>
   <si>
-    <t>ANWC117</t>
+    <t>SAM26</t>
+  </si>
+  <si>
+    <t>SAM25</t>
+  </si>
+  <si>
+    <t>SAM21</t>
+  </si>
+  <si>
+    <t>SAM20</t>
+  </si>
+  <si>
+    <t>SAM18</t>
+  </si>
+  <si>
+    <t>SAM17</t>
+  </si>
+  <si>
+    <t>SAM33</t>
+  </si>
+  <si>
+    <t>SAM16</t>
+  </si>
+  <si>
+    <t>SAM14</t>
+  </si>
+  <si>
+    <t>SAM12</t>
+  </si>
+  <si>
+    <t>SAM11</t>
+  </si>
+  <si>
+    <t>WAM58</t>
+  </si>
+  <si>
+    <t>ANWC92</t>
+  </si>
+  <si>
+    <t>ANWC90</t>
+  </si>
+  <si>
+    <t>ANWC88</t>
+  </si>
+  <si>
+    <t>SAM15</t>
+  </si>
+  <si>
+    <t>ANWC135</t>
+  </si>
+  <si>
+    <t>ANWC140</t>
+  </si>
+  <si>
+    <t>ANWC129</t>
+  </si>
+  <si>
+    <t>ANWC131</t>
+  </si>
+  <si>
+    <t>ANWC130</t>
+  </si>
+  <si>
+    <t>ANWC152</t>
+  </si>
+  <si>
+    <t>SAM35</t>
+  </si>
+  <si>
+    <t>ANWC159</t>
   </si>
   <si>
     <t>ANWC118</t>
@@ -83,67 +152,139 @@
     <t>ANWC119</t>
   </si>
   <si>
+    <t>ANWC84</t>
+  </si>
+  <si>
+    <t>ANWC94</t>
+  </si>
+  <si>
+    <t>ANWC133</t>
+  </si>
+  <si>
+    <t>ANWC136</t>
+  </si>
+  <si>
+    <t>SAM31</t>
+  </si>
+  <si>
+    <t>ANWC156</t>
+  </si>
+  <si>
+    <t>ANWC79</t>
+  </si>
+  <si>
+    <t>ANWC132</t>
+  </si>
+  <si>
+    <t>ANWC103</t>
+  </si>
+  <si>
+    <t>ANWC105</t>
+  </si>
+  <si>
+    <t>SAM32</t>
+  </si>
+  <si>
+    <t>ANWC100</t>
+  </si>
+  <si>
+    <t>SAM39</t>
+  </si>
+  <si>
+    <t>ANWC102</t>
+  </si>
+  <si>
+    <t>ANWC138</t>
+  </si>
+  <si>
+    <t>ANWC104</t>
+  </si>
+  <si>
+    <t>ANWC168</t>
+  </si>
+  <si>
+    <t>ANWC117</t>
+  </si>
+  <si>
+    <t>ANWC101</t>
+  </si>
+  <si>
+    <t>ANWC69</t>
+  </si>
+  <si>
+    <t>ANWC75</t>
+  </si>
+  <si>
+    <t>ANWC154</t>
+  </si>
+  <si>
+    <t>ANWC106</t>
+  </si>
+  <si>
+    <t>ANWC108</t>
+  </si>
+  <si>
+    <t>ANWC112</t>
+  </si>
+  <si>
+    <t>ANWC107</t>
+  </si>
+  <si>
     <t>ANWC126</t>
+  </si>
+  <si>
+    <t>SAM45</t>
+  </si>
+  <si>
+    <t>ANWC110</t>
+  </si>
+  <si>
+    <t>ANWC85</t>
+  </si>
+  <si>
+    <t>ANWC115</t>
+  </si>
+  <si>
+    <t>ANWC137</t>
+  </si>
+  <si>
+    <t>ANWC66</t>
+  </si>
+  <si>
+    <t>ANWC116</t>
+  </si>
+  <si>
+    <t>ANWC139</t>
+  </si>
+  <si>
+    <t>SAM19</t>
+  </si>
+  <si>
+    <t>ANWC141</t>
   </si>
   <si>
     <t>ANWC128</t>
   </si>
   <si>
-    <t>ANWC129</t>
-  </si>
-  <si>
-    <t>ANWC130</t>
-  </si>
-  <si>
-    <t>ANWC131</t>
-  </si>
-  <si>
-    <t>ANWC132</t>
-  </si>
-  <si>
-    <t>ANWC133</t>
-  </si>
-  <si>
-    <t>ANWC134</t>
-  </si>
-  <si>
-    <t>ANWC135</t>
-  </si>
-  <si>
-    <t>ANWC136</t>
-  </si>
-  <si>
-    <t>ANWC137</t>
-  </si>
-  <si>
-    <t>ANWC138</t>
-  </si>
-  <si>
-    <t>ANWC139</t>
-  </si>
-  <si>
-    <t>ANWC140</t>
-  </si>
-  <si>
-    <t>ANWC141</t>
-  </si>
-  <si>
     <t>ANWC142</t>
   </si>
   <si>
-    <t>ANWC143</t>
+    <t>ANWC147</t>
   </si>
   <si>
-    <t>ANWC144</t>
+    <t>ANWC109</t>
   </si>
   <si>
-    <t>ANWC145</t>
+    <t>ANWC77</t>
+  </si>
+  <si>
+    <t>ANWC162</t>
   </si>
   <si>
     <t>ANWC146</t>
   </si>
   <si>
-    <t>ANWC147</t>
+    <t>SAM34</t>
   </si>
   <si>
     <t>ANWC148</t>
@@ -152,22 +293,25 @@
     <t>ANWC150</t>
   </si>
   <si>
+    <t>ANWC145</t>
+  </si>
+  <si>
     <t>ANWC151</t>
   </si>
   <si>
-    <t>ANWC152</t>
+    <t>ANWC113</t>
   </si>
   <si>
     <t>ANWC153</t>
   </si>
   <si>
-    <t>ANWC154</t>
-  </si>
-  <si>
     <t>ANWC155</t>
   </si>
   <si>
-    <t>ANWC156</t>
+    <t>SAM37</t>
+  </si>
+  <si>
+    <t>ANWC71</t>
   </si>
   <si>
     <t>ANWC157</t>
@@ -176,7 +320,7 @@
     <t>ANWC158</t>
   </si>
   <si>
-    <t>ANWC159</t>
+    <t>ANWC143</t>
   </si>
   <si>
     <t>ANWC160</t>
@@ -185,31 +329,10 @@
     <t>ANWC161</t>
   </si>
   <si>
-    <t>ANWC162</t>
-  </si>
-  <si>
-    <t>ANWC163</t>
-  </si>
-  <si>
-    <t>ANWC168</t>
-  </si>
-  <si>
     <t>ANWC170</t>
   </si>
   <si>
-    <t>ANWC66</t>
-  </si>
-  <si>
-    <t>ANWC67</t>
-  </si>
-  <si>
     <t>ANWC68</t>
-  </si>
-  <si>
-    <t>ANWC69</t>
-  </si>
-  <si>
-    <t>ANWC71</t>
   </si>
   <si>
     <t>ANWC72</t>
@@ -218,154 +341,31 @@
     <t>ANWC73</t>
   </si>
   <si>
-    <t>ANWC75</t>
+    <t>ANWC134</t>
   </si>
   <si>
-    <t>ANWC77</t>
+    <t>ANWC67</t>
+  </si>
+  <si>
+    <t>ANWC81</t>
+  </si>
+  <si>
+    <t>ANWC163</t>
+  </si>
+  <si>
+    <t>WAM59</t>
   </si>
   <si>
     <t>ANWC78</t>
   </si>
   <si>
-    <t>ANWC79</t>
+    <t>SAM38</t>
+  </si>
+  <si>
+    <t>ANWC144</t>
   </si>
   <si>
     <t>ANWC80</t>
-  </si>
-  <si>
-    <t>ANWC81</t>
-  </si>
-  <si>
-    <t>ANWC84</t>
-  </si>
-  <si>
-    <t>ANWC85</t>
-  </si>
-  <si>
-    <t>ANWC88</t>
-  </si>
-  <si>
-    <t>ANWC90</t>
-  </si>
-  <si>
-    <t>ANWC92</t>
-  </si>
-  <si>
-    <t>ANWC94</t>
-  </si>
-  <si>
-    <t>SAM11</t>
-  </si>
-  <si>
-    <t>SAM12</t>
-  </si>
-  <si>
-    <t>SAM14</t>
-  </si>
-  <si>
-    <t>SAM15</t>
-  </si>
-  <si>
-    <t>SAM16</t>
-  </si>
-  <si>
-    <t>SAM17</t>
-  </si>
-  <si>
-    <t>SAM18</t>
-  </si>
-  <si>
-    <t>SAM19</t>
-  </si>
-  <si>
-    <t>SAM20</t>
-  </si>
-  <si>
-    <t>SAM21</t>
-  </si>
-  <si>
-    <t>SAM25</t>
-  </si>
-  <si>
-    <t>SAM26</t>
-  </si>
-  <si>
-    <t>SAM27</t>
-  </si>
-  <si>
-    <t>SAM28</t>
-  </si>
-  <si>
-    <t>SAM29</t>
-  </si>
-  <si>
-    <t>SAM30</t>
-  </si>
-  <si>
-    <t>SAM31</t>
-  </si>
-  <si>
-    <t>SAM32</t>
-  </si>
-  <si>
-    <t>SAM33</t>
-  </si>
-  <si>
-    <t>SAM34</t>
-  </si>
-  <si>
-    <t>SAM35</t>
-  </si>
-  <si>
-    <t>SAM36</t>
-  </si>
-  <si>
-    <t>SAM37</t>
-  </si>
-  <si>
-    <t>SAM38</t>
-  </si>
-  <si>
-    <t>SAM39</t>
-  </si>
-  <si>
-    <t>SAM41</t>
-  </si>
-  <si>
-    <t>SAM44</t>
-  </si>
-  <si>
-    <t>SAM45</t>
-  </si>
-  <si>
-    <t>SAM46</t>
-  </si>
-  <si>
-    <t>SAM8</t>
-  </si>
-  <si>
-    <t>WAM55</t>
-  </si>
-  <si>
-    <t>WAM56</t>
-  </si>
-  <si>
-    <t>WAM57</t>
-  </si>
-  <si>
-    <t>WAM58</t>
-  </si>
-  <si>
-    <t>WAM59</t>
-  </si>
-  <si>
-    <t>WAM60</t>
-  </si>
-  <si>
-    <t>WAM63</t>
-  </si>
-  <si>
-    <t>WAM64</t>
   </si>
 </sst>
 </file>
@@ -383,7 +383,9 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Lucida Grande"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -690,7 +692,7 @@
   <dimension ref="A1:DJ114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>